<commit_message>
add images and listviw PO
</commit_message>
<xml_diff>
--- a/doc/code_standards/Code_Standards.xlsx
+++ b/doc/code_standards/Code_Standards.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hades/Documents/GitHub/AndroidAboutDemos/doc/code_standards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741A218E-819F-B143-84DC-D5D922E3BB72}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054B806C-84B3-5D4A-80B3-881D4F463FFF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{7476E77F-5092-004B-9FED-6DC65910482C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ref" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="58">
   <si>
     <t>Category</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -46,10 +47,6 @@
   </si>
   <si>
     <t>Version</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bitmap</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -128,14 +125,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Create drawable from a bitmap(resource display metrics)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remote image has small,middle,large,etc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Memoey cache &gt; Disk cache -&gt; Network</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -146,6 +135,167 @@
   <si>
     <t>Memoey cache = LruCache + SoftReference
 LruCache =&gt; SoftReference</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ListView</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create drawable from a bitmap (resource display metrics)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ViewHolder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if (convertView == null) {
+    convertView.setTag(viewHolder);
+}
+else{}
+    viewHolder = (ViewHolder) convertView.getTag()
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use convertView tag  to cache ViewHolder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.9.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Choose image format</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WebP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Image</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Determine optimal quality values using Scalar values(JPG and WebP only),such as Butteraugli.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Serving sizess:
+Remote store multiple sizes of images,
+but serve one appropriate size </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SVG
+WebP
+PNG: transparency and non-transparency but simple,
+JPG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-
+&gt;=4.2.1(17)
+-
+-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SVG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SVG:
+1. PNG generation
+1) VectorDrawable
+Android &gt;= 5.0(21), full support
+Android &lt;=4.4(20), Subset supported
+2) SVG:Android gradle plugin &gt;= 1.5
+PSD: Android Studio &gt;=2.2 
+------------------------
+2. Support library
+1) support library &gt;= 23.2
+   Supprot android &gt;=2.1(7)
+2) Android gradle plugin &gt;= 2.0
+3) VectorDrawableCompat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Convert imges tto Webp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;=4.2.1(17)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Label</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Network xfer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adapter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Link</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://developer.android.google.cn/topic/performance/network-xfer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reducing image download sizes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://developer.android.google.cn/studio/write/vector-asset-studio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://developer.android.google.cn/studio/write/convert-webp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://developer.android.google.cn/guide/topics/graphics/vector-drawable-resources</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://developer.android.google.cn/topic/performance/graphics/cache-bitmap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Caching Bitmaps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Load bitmap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://developer.android.google.cn/topic/performance/graphics/load-bitmap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cache bit,ap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compression</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Other tols</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -153,7 +303,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -175,6 +325,15 @@
       <color theme="1"/>
       <name val="等线"/>
       <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="等线"/>
+      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -217,12 +376,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -256,8 +418,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -570,320 +742,614 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DF8FD84-0C85-AB4D-8863-F263B3E6951E}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="3"/>
-    <col min="2" max="2" width="52.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.1640625" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="13" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="3" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.1640625" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="34">
+      <c r="A2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="51">
+      <c r="A4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="34">
+      <c r="A5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="51">
+      <c r="A6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="34">
-      <c r="A2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17">
+      <c r="A8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="221">
+      <c r="A11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="51">
+      <c r="A12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="34">
+      <c r="A13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="17">
+      <c r="A14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="17">
+      <c r="A15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="B17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="51">
-      <c r="A4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="34">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="51">
-      <c r="A6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="17">
-      <c r="A8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="2">
+    <row r="19" spans="1:6" ht="102">
+      <c r="A19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6">
       <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
+      <c r="B20" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="E20" s="4"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
+      <c r="B21" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="E21" s="4"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="E22" s="4"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="E23" s="4"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="E24" s="4"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="2"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E930335-63F7-A14F-A6F0-FEB4D192F781}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="85.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="13" customFormat="1">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{02E146A9-D425-DA4B-8366-19D595915BA3}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{11F5B5B0-D03F-7B4C-8BE6-08773C1D3968}"/>
+    <hyperlink ref="C6" r:id="rId3" xr:uid="{C8047642-760A-B047-8A1F-2881C0B172E2}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{D294E976-52AE-FB4E-A0CE-7B17C7AA898E}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{5A538792-E0E3-EE49-AAFD-717FDE4CD6D5}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{97C56CAF-3D22-BF48-830D-10EF8F5F90B5}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{F6D34DD3-CBF8-334E-AAEE-211F5543133B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add rule for Non-static inner classes
</commit_message>
<xml_diff>
--- a/doc/code_standards/Code_Standards.xlsx
+++ b/doc/code_standards/Code_Standards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hades/Documents/GitHub/AndroidAboutDemos/doc/code_standards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF9019D-FF5C-C94E-A728-8CEC0AF26557}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3706BD-75B9-9F4E-B27D-F14E5186BD9E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="460" windowWidth="27840" windowHeight="17540" xr2:uid="{7476E77F-5092-004B-9FED-6DC65910482C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="62">
   <si>
     <t>Category</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -308,7 +308,12 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Inner class</t>
+    <t>Remove  an implicit reference  of non-static inner classes (Runnable/handler/loader/task/AsyncTask) 
+to their outer class(Fragment or Activity)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Non-static inner classes</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -784,7 +789,7 @@
   <cols>
     <col min="1" max="1" width="20.5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="109.5" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="3" customWidth="1"/>
     <col min="6" max="6" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -1180,17 +1185,21 @@
       <c r="E20" s="4"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" ht="34">
       <c r="A21" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="2"/>
+      <c r="F21" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="4"/>

</xml_diff>

<commit_message>
DB cont row num
</commit_message>
<xml_diff>
--- a/doc/code_standards/Code_Standards.xlsx
+++ b/doc/code_standards/Code_Standards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hades/Documents/GitHub/AndroidAboutDemos/doc/code_standards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF94024-1D55-1542-84D4-8DBFE0670CDD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFAE84B-3E41-F84A-8F73-2C817846AFCD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="460" windowWidth="27840" windowHeight="17540" xr2:uid="{7476E77F-5092-004B-9FED-6DC65910482C}"/>
   </bookViews>
@@ -858,7 +858,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>